<commit_message>
feat add requrchase check
</commit_message>
<xml_diff>
--- a/src/test/doc/meeting/1127软件修改.xlsx
+++ b/src/test/doc/meeting/1127软件修改.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">bug列表!$B$1:$H$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">bug列表!$B$1:$H$74</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="395">
   <si>
     <t>系统</t>
   </si>
@@ -1654,6 +1654,10 @@
   </si>
   <si>
     <t>购买商品-选择赠品</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>回购审批，单独的回购审批页面</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -6946,10 +6950,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="B1:H117"/>
+  <dimension ref="B1:H118"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G61" sqref="D56:G61"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.59765625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8053,7 +8057,7 @@
       <c r="B61" s="70">
         <v>42701</v>
       </c>
-      <c r="C61" s="89"/>
+      <c r="C61" s="88"/>
       <c r="D61" s="62" t="s">
         <v>357</v>
       </c>
@@ -8067,14 +8071,10 @@
       <c r="H61" s="53"/>
     </row>
     <row r="62" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="70">
-        <v>42701</v>
-      </c>
-      <c r="C62" s="87" t="s">
-        <v>358</v>
-      </c>
+      <c r="B62" s="70"/>
+      <c r="C62" s="89"/>
       <c r="D62" s="62" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
       <c r="E62" s="53" t="s">
         <v>320</v>
@@ -8082,21 +8082,21 @@
       <c r="F62" s="53" t="s">
         <v>381</v>
       </c>
-      <c r="G62" s="53" t="s">
-        <v>223</v>
-      </c>
+      <c r="G62" s="53"/>
       <c r="H62" s="53"/>
     </row>
     <row r="63" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="70">
         <v>42701</v>
       </c>
-      <c r="C63" s="89"/>
+      <c r="C63" s="87" t="s">
+        <v>358</v>
+      </c>
       <c r="D63" s="62" t="s">
-        <v>359</v>
+        <v>386</v>
       </c>
       <c r="E63" s="53" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F63" s="53" t="s">
         <v>381</v>
@@ -8106,51 +8106,55 @@
       </c>
       <c r="H63" s="53"/>
     </row>
-    <row r="64" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="70">
         <v>42701</v>
       </c>
-      <c r="C64" s="78" t="s">
-        <v>360</v>
-      </c>
+      <c r="C64" s="89"/>
       <c r="D64" s="62" t="s">
-        <v>392</v>
+        <v>359</v>
       </c>
       <c r="E64" s="53" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="F64" s="53" t="s">
         <v>381</v>
       </c>
       <c r="G64" s="53" t="s">
-        <v>387</v>
+        <v>223</v>
       </c>
       <c r="H64" s="53"/>
     </row>
-    <row r="65" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="70">
         <v>42701</v>
       </c>
-      <c r="C65" s="87" t="s">
-        <v>361</v>
+      <c r="C65" s="78" t="s">
+        <v>360</v>
       </c>
       <c r="D65" s="62" t="s">
-        <v>362</v>
+        <v>392</v>
       </c>
       <c r="E65" s="53" t="s">
-        <v>322</v>
-      </c>
-      <c r="F65" s="53"/>
-      <c r="G65" s="53"/>
+        <v>320</v>
+      </c>
+      <c r="F65" s="53" t="s">
+        <v>381</v>
+      </c>
+      <c r="G65" s="53" t="s">
+        <v>387</v>
+      </c>
       <c r="H65" s="53"/>
     </row>
-    <row r="66" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="70">
         <v>42701</v>
       </c>
-      <c r="C66" s="88"/>
+      <c r="C66" s="87" t="s">
+        <v>361</v>
+      </c>
       <c r="D66" s="62" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E66" s="53" t="s">
         <v>322</v>
@@ -8159,13 +8163,13 @@
       <c r="G66" s="53"/>
       <c r="H66" s="53"/>
     </row>
-    <row r="67" spans="2:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="70">
         <v>42701</v>
       </c>
       <c r="C67" s="88"/>
       <c r="D67" s="62" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E67" s="53" t="s">
         <v>322</v>
@@ -8174,13 +8178,13 @@
       <c r="G67" s="53"/>
       <c r="H67" s="53"/>
     </row>
-    <row r="68" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="70">
         <v>42701</v>
       </c>
       <c r="C68" s="88"/>
       <c r="D68" s="62" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E68" s="53" t="s">
         <v>322</v>
@@ -8189,13 +8193,13 @@
       <c r="G68" s="53"/>
       <c r="H68" s="53"/>
     </row>
-    <row r="69" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="70">
         <v>42701</v>
       </c>
       <c r="C69" s="88"/>
       <c r="D69" s="62" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E69" s="53" t="s">
         <v>322</v>
@@ -8210,7 +8214,7 @@
       </c>
       <c r="C70" s="88"/>
       <c r="D70" s="62" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E70" s="53" t="s">
         <v>322</v>
@@ -8223,9 +8227,9 @@
       <c r="B71" s="70">
         <v>42701</v>
       </c>
-      <c r="C71" s="89"/>
+      <c r="C71" s="88"/>
       <c r="D71" s="62" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E71" s="53" t="s">
         <v>322</v>
@@ -8234,15 +8238,13 @@
       <c r="G71" s="53"/>
       <c r="H71" s="53"/>
     </row>
-    <row r="72" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="70">
         <v>42701</v>
       </c>
-      <c r="C72" s="78" t="s">
-        <v>369</v>
-      </c>
+      <c r="C72" s="89"/>
       <c r="D72" s="62" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="E72" s="53" t="s">
         <v>322</v>
@@ -8251,15 +8253,15 @@
       <c r="G72" s="53"/>
       <c r="H72" s="53"/>
     </row>
-    <row r="73" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="70">
         <v>42701</v>
       </c>
       <c r="C73" s="78" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D73" s="62" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E73" s="53" t="s">
         <v>322</v>
@@ -8269,10 +8271,18 @@
       <c r="H73" s="53"/>
     </row>
     <row r="74" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="65"/>
-      <c r="C74" s="78"/>
-      <c r="D74" s="62"/>
-      <c r="E74" s="53"/>
+      <c r="B74" s="70">
+        <v>42701</v>
+      </c>
+      <c r="C74" s="78" t="s">
+        <v>370</v>
+      </c>
+      <c r="D74" s="62" t="s">
+        <v>371</v>
+      </c>
+      <c r="E74" s="53" t="s">
+        <v>322</v>
+      </c>
       <c r="F74" s="53"/>
       <c r="G74" s="53"/>
       <c r="H74" s="53"/>
@@ -8295,7 +8305,7 @@
       <c r="G76" s="53"/>
       <c r="H76" s="53"/>
     </row>
-    <row r="77" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="65"/>
       <c r="C77" s="78"/>
       <c r="D77" s="62"/>
@@ -8664,9 +8674,18 @@
       <c r="G117" s="53"/>
       <c r="H117" s="53"/>
     </row>
+    <row r="118" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B118" s="65"/>
+      <c r="C118" s="78"/>
+      <c r="D118" s="62"/>
+      <c r="E118" s="53"/>
+      <c r="F118" s="53"/>
+      <c r="G118" s="53"/>
+      <c r="H118" s="53"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C65:C71"/>
+    <mergeCell ref="C66:C72"/>
     <mergeCell ref="C33:C35"/>
     <mergeCell ref="C37:C39"/>
     <mergeCell ref="C40:C41"/>
@@ -8675,18 +8694,18 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C56:C61"/>
-    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C56:C62"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H74:H117">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H75:H118">
       <formula1>"未完成,进行中,已完成"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E73 F2:F43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E74 F2:F43">
       <formula1>"易用性,新功能"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G73">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G74">
       <formula1>"已完成,未完成"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>